<commit_message>
saco acentos de los TCs
</commit_message>
<xml_diff>
--- a/SuraClaims/Anular Pago Siniestro.xlsx
+++ b/SuraClaims/Anular Pago Siniestro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD444DE-F95E-4A27-97EE-B198DE15E542}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFBAB77-E455-4B51-BC8B-CFA45E298121}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF74D057-6E01-4208-A115-80971374A007}"/>
   </bookViews>
@@ -48,15 +48,9 @@
     <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
   </si>
   <si>
-    <t>rherner</t>
-  </si>
-  <si>
     <t>silverarrow</t>
   </si>
   <si>
-    <t>04104015648</t>
-  </si>
-  <si>
     <t>tcorvetto</t>
   </si>
   <si>
@@ -70,6 +64,12 @@
   </si>
   <si>
     <t xml:space="preserve">1120170200908 </t>
+  </si>
+  <si>
+    <t>1120194100405</t>
+  </si>
+  <si>
+    <t>apellegrini</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -483,13 +483,13 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -497,19 +497,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio item de opcion reclamo en generar inspeccion. Agrego screenshots a scripts varios
</commit_message>
<xml_diff>
--- a/SuraClaims/Anular Pago Siniestro.xlsx
+++ b/SuraClaims/Anular Pago Siniestro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFBAB77-E455-4B51-BC8B-CFA45E298121}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3668CC07-B976-46AD-BBC4-DA8CEA005EBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF74D057-6E01-4208-A115-80971374A007}"/>
   </bookViews>
@@ -66,10 +66,10 @@
     <t xml:space="preserve">1120170200908 </t>
   </si>
   <si>
-    <t>1120194100405</t>
-  </si>
-  <si>
     <t>apellegrini</t>
+  </si>
+  <si>
+    <t>1220194200662</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,13 +483,13 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
arreglo menu lateral - datos financieros
</commit_message>
<xml_diff>
--- a/SuraClaims/Anular Pago Siniestro.xlsx
+++ b/SuraClaims/Anular Pago Siniestro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3668CC07-B976-46AD-BBC4-DA8CEA005EBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97D2804-9899-46DD-AF2F-3503CAC62F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF74D057-6E01-4208-A115-80971374A007}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -69,7 +69,13 @@
     <t>apellegrini</t>
   </si>
   <si>
-    <t>1220194200662</t>
+    <t>1120194100412</t>
+  </si>
+  <si>
+    <t>1220194200667</t>
+  </si>
+  <si>
+    <t>0420194406717</t>
   </si>
 </sst>
 </file>
@@ -444,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA01E7D-480B-457E-89FE-07C13B233011}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,26 +495,60 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
agrego número de orden de pago en la validación de pagos en SISE
</commit_message>
<xml_diff>
--- a/SuraClaims/Anular Pago Siniestro.xlsx
+++ b/SuraClaims/Anular Pago Siniestro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97D2804-9899-46DD-AF2F-3503CAC62F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A40276-3625-41C2-B333-FDD6757997FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF74D057-6E01-4208-A115-80971374A007}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -63,9 +63,6 @@
     <t>NroSiniestro</t>
   </si>
   <si>
-    <t xml:space="preserve">1120170200908 </t>
-  </si>
-  <si>
     <t>apellegrini</t>
   </si>
   <si>
@@ -76,6 +73,15 @@
   </si>
   <si>
     <t>0420194406717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0420172008483 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1220170301429 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1120170200936 </t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA01E7D-480B-457E-89FE-07C13B233011}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,13 +495,13 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -506,13 +512,13 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -523,13 +529,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -549,7 +555,41 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agrego en el test case de anulación dos smart folders (una para anular en sí y otra para obtener el número de anulación)
</commit_message>
<xml_diff>
--- a/SuraClaims/Anular Pago Siniestro.xlsx
+++ b/SuraClaims/Anular Pago Siniestro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A40276-3625-41C2-B333-FDD6757997FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02840D2-5F0D-4220-B061-4BB3305A2476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF74D057-6E01-4208-A115-80971374A007}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -51,9 +51,6 @@
     <t>silverarrow</t>
   </si>
   <si>
-    <t>tcorvetto</t>
-  </si>
-  <si>
     <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
   </si>
   <si>
@@ -66,22 +63,31 @@
     <t>apellegrini</t>
   </si>
   <si>
-    <t>1120194100412</t>
-  </si>
-  <si>
-    <t>1220194200667</t>
-  </si>
-  <si>
-    <t>0420194406717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0420172008483 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1220170301429 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1120170200936 </t>
+    <t>0420194406830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1120194100442 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1220194200684 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1220170301442 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1120170200942 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0420172008629 </t>
+  </si>
+  <si>
+    <t>Acción</t>
+  </si>
+  <si>
+    <t>Anular</t>
+  </si>
+  <si>
+    <t>Obtener número</t>
   </si>
 </sst>
 </file>
@@ -456,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA01E7D-480B-457E-89FE-07C13B233011}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A7"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,10 +487,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -495,16 +504,16 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -512,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -521,7 +530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -529,44 +538,44 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -574,22 +583,42 @@
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrección de error behavior en los test case
</commit_message>
<xml_diff>
--- a/SuraClaims/Anular Pago Siniestro.xlsx
+++ b/SuraClaims/Anular Pago Siniestro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02840D2-5F0D-4220-B061-4BB3305A2476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8BF8F4-B3C4-429D-9497-7632EABA6C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF74D057-6E01-4208-A115-80971374A007}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -66,21 +66,6 @@
     <t>0420194406830</t>
   </si>
   <si>
-    <t xml:space="preserve">1120194100442 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1220194200684 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1220170301442 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1120170200942 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0420172008629 </t>
-  </si>
-  <si>
     <t>Acción</t>
   </si>
   <si>
@@ -88,6 +73,21 @@
   </si>
   <si>
     <t>Obtener número</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0420172010228 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1120170200969 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1220170301466 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1120194100448 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1220194200694  </t>
   </si>
 </sst>
 </file>
@@ -144,10 +144,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA01E7D-480B-457E-89FE-07C13B233011}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +491,7 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -527,7 +528,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,7 +545,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -560,11 +561,11 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -580,11 +581,11 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -600,8 +601,11 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>16</v>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -617,7 +621,50 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>